<commit_message>
added different seeds for few shot comb nlpcc
</commit_message>
<xml_diff>
--- a/big_results.xlsx
+++ b/big_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="140">
   <si>
     <t>model_base</t>
   </si>
@@ -124,15 +124,36 @@
     <t>hash</t>
   </si>
   <si>
+    <t>random_seed</t>
+  </si>
+  <si>
     <t>microsoft/infoxlm-base</t>
   </si>
   <si>
     <t>['arc', 'argmin', 'fnc1', 'iac1', 'ibmcs', 'perspectrum', 'semeval2016t6', 'snopes', 'twitter2015', 'twitter2017', 'vast']</t>
   </si>
   <si>
+    <t>['arc', 'argmin', 'fnc1', 'iac1', 'ibmcs', 'perspectrum', 'semeval2016t6', 'snopes', 'twitter2015', 'twitter2017', 'vast', 'comb_nlpcc_5']</t>
+  </si>
+  <si>
+    <t>['arc', 'argmin', 'fnc1', 'iac1', 'ibmcs', 'perspectrum', 'semeval2016t6', 'snopes', 'twitter2015', 'twitter2017', 'vast', 'comb_nlpcc_32']</t>
+  </si>
+  <si>
+    <t>['arc', 'argmin', 'fnc1', 'iac1', 'ibmcs', 'perspectrum', 'semeval2016t6', 'snopes', 'twitter2015', 'twitter2017', 'vast', 'comb_nlpcc_128']</t>
+  </si>
+  <si>
+    <t>['arc', 'argmin', 'fnc1', 'iac1', 'ibmcs', 'perspectrum', 'semeval2016t6', 'snopes', 'twitter2015', 'twitter2017', 'vast', 'comb_nlpcc_256']</t>
+  </si>
+  <si>
     <t>stance_3</t>
   </si>
   <si>
+    <t>stance_0</t>
+  </si>
+  <si>
+    <t>senti-stance</t>
+  </si>
+  <si>
     <t>equal</t>
   </si>
   <si>
@@ -211,6 +232,78 @@
     <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-attempt_r5/checkpoint-best</t>
   </si>
   <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r1/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r2/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r3/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r4/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-attempt_r5/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-ld_mldoc-extra_mlm-amazonzh-variant_3-attempt_r0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-ld_mldoc-extra_mlm-amazonzh-variant_3-attempt_r1/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-ld_mldoc-extra_mlm-amazonzh-variant_3-attempt_r2/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-ld_mldoc-extra_mlm-amazonzh-variant_3-attempt_r3/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-ld_mldoc-extra_mlm-amazonzh-variant_3-attempt_r4/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../senti-stance/outputs/senti-stance_expt-r0/checkpoint-best/</t>
+  </si>
+  <si>
+    <t>../senti-stance/outputs/senti-stance_expt-r1/checkpoint-best/</t>
+  </si>
+  <si>
+    <t>../senti-stance/outputs/senti-stance_expt-r2/checkpoint-best/</t>
+  </si>
+  <si>
+    <t>../senti-stance/outputs/senti-stance_expt-r3/checkpoint-best/</t>
+  </si>
+  <si>
+    <t>../senti-stance/outputs/senti-stance_expt-r4/checkpoint-best/</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs5-attempt_0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs32-attempt_0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs128-attempt_0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs256-attempt_0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs5-attempt_r0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs32-attempt_r0/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs5-attempt_r2/checkpoint-best</t>
+  </si>
+  <si>
+    <t>../stance_expts/ml-stance-11_en-no_mlm-2_neg-rs_rp-variant_3-fs5-attempt_r1/checkpoint-best</t>
+  </si>
+  <si>
     <t>fd6ee81ee999aa9e844bce113233547d33e8e4c8994a0ca88ff563fef9b48851</t>
   </si>
   <si>
@@ -269,6 +362,78 @@
   </si>
   <si>
     <t>e7025f1b4497bfc7d6a4b1035dea324632d623396d580ce70714b826e4df5bac</t>
+  </si>
+  <si>
+    <t>af09d38867693e4016addc04e068c1f9928d009190de9b55b20b29a4cb438670</t>
+  </si>
+  <si>
+    <t>92ac6249c339deec5e54d73eab8af01f1f00e8f9cb48edc3fd999107637edf1d</t>
+  </si>
+  <si>
+    <t>194cc889e3d41e747582c6f138ff0e8e460d1210729a3a69bb800ad82511163b</t>
+  </si>
+  <si>
+    <t>b247c7dbc718bc7dba1de426f654208932d4bfab2fd5a2e61895297d66e29fc3</t>
+  </si>
+  <si>
+    <t>80dc049cb201cb64bcabd100b390f114d6e98ef9a0f77c2455adb2865e024b7b</t>
+  </si>
+  <si>
+    <t>d9511fe22cd096f9e156f74eaa7123abb4619647742796af43726603b483efd5</t>
+  </si>
+  <si>
+    <t>08f42f8dea509b8a368eb92df97fd2a35c73d1e71abd80e9225a84edf406394a</t>
+  </si>
+  <si>
+    <t>aca95d98052d6f2433031d40b027eb42ecf329030bc7e2d801dd9a8304667a39</t>
+  </si>
+  <si>
+    <t>95fd4e246cee80f3dda1b8e7ad85b195cae431bc137d2c5fb1db91b74bb0995e</t>
+  </si>
+  <si>
+    <t>f306366a7e9c15f2ca35473c798a2a560cce1b3deae4bfec4d4971b6264984aa</t>
+  </si>
+  <si>
+    <t>39ed52c21cdac807d16878016ebe0e00f3ecf7b9ab5e6337a858edff3d53fe71</t>
+  </si>
+  <si>
+    <t>748ac50f9f4b304afffc0a961dcb05ddd97188b970e76e24257d450af83582be</t>
+  </si>
+  <si>
+    <t>559d03230475e4559bf51ba18a898d2ff78e6d7ca2d61eccd829a0f231b1d075</t>
+  </si>
+  <si>
+    <t>2687b97c540f03ed9ddbc1143d4133a68ee5494f556047666481507aebc5f1cf</t>
+  </si>
+  <si>
+    <t>8e92accbabc71f06f077b2e9a5512c0379b7c468604dcaf222f1fa5b20031c4d</t>
+  </si>
+  <si>
+    <t>f464c8e5f3264ed6dc150e1bb6874fefbbf14e85265c2ec7c665a361fa5651cc</t>
+  </si>
+  <si>
+    <t>74b9066e604de94398aa8c9705719122ad49a33fde005e5b879322b71ec0af39</t>
+  </si>
+  <si>
+    <t>50f79fcd52604ec0d09e3865fbc93703fc1c5fc03c76acfbb25883586993f91e</t>
+  </si>
+  <si>
+    <t>b9ead73e2d77899b05fe6fc497ad33c989054e7d27fee0ec12fe6963339be8aa</t>
+  </si>
+  <si>
+    <t>7b27b000bc70707aacdd24e96795eadeb00f3002c63d070441f82bb842486924</t>
+  </si>
+  <si>
+    <t>7e5cd4db42d55ddc14dbec9bf82bbc19b2749460e5e01e5ec74d4fa882d1d072</t>
+  </si>
+  <si>
+    <t>3f4228a6f7b4f2701ff1f80c6d315c74d35a012d4e06464b2200bb1f9eb68489</t>
+  </si>
+  <si>
+    <t>09e184713efea0d31ce5a12d31ca9a85e213d985d2060bd7f685fb631c415d3d</t>
+  </si>
+  <si>
+    <t>25549606c3fbfa3808ce744416defa1f81efa4c550bb0c29ad82b43e30de5ef6</t>
   </si>
 </sst>
 </file>
@@ -626,13 +791,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,16 +906,19 @@
       <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>128</v>
@@ -768,13 +936,13 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J2">
         <v>0.3</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L2">
         <v>0.01</v>
@@ -795,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="T2" t="b">
         <v>0</v>
@@ -804,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -834,21 +1002,21 @@
         <v>0.586876838814128</v>
       </c>
       <c r="AI2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="AJ2" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>128</v>
@@ -866,13 +1034,13 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J3">
         <v>0.3</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L3">
         <v>0.01</v>
@@ -893,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="T3" t="b">
         <v>0</v>
@@ -902,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -932,21 +1100,21 @@
         <v>0.5406144299719992</v>
       </c>
       <c r="AI3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="AJ3" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>128</v>
@@ -964,13 +1132,13 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J4">
         <v>0.3</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L4">
         <v>0.01</v>
@@ -991,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="T4" t="b">
         <v>0</v>
@@ -1000,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -1030,21 +1198,21 @@
         <v>0.5667721825824592</v>
       </c>
       <c r="AI4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="AJ4" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>128</v>
@@ -1062,13 +1230,13 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J5">
         <v>0.3</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>0.01</v>
@@ -1089,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="T5" t="b">
         <v>0</v>
@@ -1098,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
@@ -1131,21 +1299,21 @@
         <v>0.6045533966268596</v>
       </c>
       <c r="AI5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="AJ5" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>128</v>
@@ -1163,13 +1331,13 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J6">
         <v>0.3</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L6">
         <v>0.01</v>
@@ -1190,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="T6" t="b">
         <v>0</v>
@@ -1199,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W6" t="b">
         <v>0</v>
@@ -1232,21 +1400,21 @@
         <v>0.5962915173237754</v>
       </c>
       <c r="AI6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AJ6" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>128</v>
@@ -1264,13 +1432,13 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J7">
         <v>0.3</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L7">
         <v>0.01</v>
@@ -1291,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="S7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="T7" t="b">
         <v>0</v>
@@ -1300,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W7" t="b">
         <v>0</v>
@@ -1333,21 +1501,21 @@
         <v>0.548275033369672</v>
       </c>
       <c r="AI7" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="AJ7" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>128</v>
@@ -1365,13 +1533,13 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J8">
         <v>0.3</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L8">
         <v>0.01</v>
@@ -1392,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="T8" t="b">
         <v>0</v>
@@ -1401,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W8" t="b">
         <v>0</v>
@@ -1434,21 +1602,21 @@
         <v>0.5992932797694498</v>
       </c>
       <c r="AI8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="AJ8" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>128</v>
@@ -1466,13 +1634,13 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J9">
         <v>0.3</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L9">
         <v>0.01</v>
@@ -1493,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="S9" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="T9" t="b">
         <v>0</v>
@@ -1502,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W9" t="b">
         <v>0</v>
@@ -1535,21 +1703,21 @@
         <v>0.6024706091886282</v>
       </c>
       <c r="AI9" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AJ9" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>128</v>
@@ -1567,13 +1735,13 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J10">
         <v>0.3</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L10">
         <v>0.01</v>
@@ -1600,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W10" t="b">
         <v>0</v>
@@ -1609,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="Y10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z10">
         <v>16</v>
@@ -1636,21 +1804,21 @@
         <v>0.5967769542168483</v>
       </c>
       <c r="AI10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="AJ10" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>128</v>
@@ -1668,13 +1836,13 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J11">
         <v>0.3</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L11">
         <v>0.01</v>
@@ -1701,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W11" t="b">
         <v>0</v>
@@ -1710,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="Y11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z11">
         <v>16</v>
@@ -1737,21 +1905,21 @@
         <v>0.5515704454402147</v>
       </c>
       <c r="AI11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="AJ11" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>128</v>
@@ -1769,13 +1937,13 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J12">
         <v>0.3</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>0.01</v>
@@ -1802,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -1811,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="Y12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z12">
         <v>16</v>
@@ -1838,21 +2006,21 @@
         <v>0.552774178025092</v>
       </c>
       <c r="AI12" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="AJ12" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>128</v>
@@ -1870,13 +2038,13 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J13">
         <v>0.3</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L13">
         <v>0.01</v>
@@ -1903,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -1912,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="Y13" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z13">
         <v>16</v>
@@ -1939,21 +2107,21 @@
         <v>0.5592074033081228</v>
       </c>
       <c r="AI13" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AJ13" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>128</v>
@@ -1971,13 +2139,13 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J14">
         <v>0.3</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L14">
         <v>0.01</v>
@@ -2004,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W14" t="b">
         <v>0</v>
@@ -2013,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="Y14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z14">
         <v>16</v>
@@ -2040,21 +2208,21 @@
         <v>0.5417429045080056</v>
       </c>
       <c r="AI14" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AJ14" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>128</v>
@@ -2072,13 +2240,13 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J15">
         <v>0.3</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L15">
         <v>0.01</v>
@@ -2105,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="V15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W15" t="b">
         <v>0</v>
@@ -2114,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="Y15" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="Z15">
         <v>16</v>
@@ -2141,21 +2309,21 @@
         <v>0.5698282299315306</v>
       </c>
       <c r="AI15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="AJ15" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>128</v>
@@ -2173,13 +2341,13 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J16">
         <v>0.3</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L16">
         <v>0.01</v>
@@ -2206,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="V16" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
@@ -2239,21 +2407,21 @@
         <v>0.5810215530620623</v>
       </c>
       <c r="AI16" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="AJ16" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>128</v>
@@ -2271,13 +2439,13 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J17">
         <v>0.3</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L17">
         <v>0.01</v>
@@ -2304,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="V17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W17" t="b">
         <v>0</v>
@@ -2337,21 +2505,21 @@
         <v>0.5783794487705053</v>
       </c>
       <c r="AI17" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="AJ17" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>128</v>
@@ -2369,13 +2537,13 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J18">
         <v>0.3</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L18">
         <v>0.01</v>
@@ -2402,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W18" t="b">
         <v>0</v>
@@ -2435,21 +2603,21 @@
         <v>0.5725829868609268</v>
       </c>
       <c r="AI18" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AJ18" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>128</v>
@@ -2467,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J19">
         <v>0.3</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L19">
         <v>0.01</v>
@@ -2500,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W19" t="b">
         <v>0</v>
@@ -2533,21 +2701,21 @@
         <v>0.5874730493255385</v>
       </c>
       <c r="AI19" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="AJ19" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>128</v>
@@ -2565,13 +2733,13 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J20">
         <v>0.3</v>
       </c>
       <c r="K20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>0.01</v>
@@ -2598,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2631,21 +2799,21 @@
         <v>0.5743165918991666</v>
       </c>
       <c r="AI20" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="AJ20" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>128</v>
@@ -2663,13 +2831,13 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J21">
         <v>0.3</v>
       </c>
       <c r="K21" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="L21">
         <v>0.01</v>
@@ -2696,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="V21" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="W21" t="b">
         <v>0</v>
@@ -2729,10 +2897,2344 @@
         <v>0.5807680174366916</v>
       </c>
       <c r="AI21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="AJ21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
+        <v>128</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.105</v>
+      </c>
+      <c r="G22">
+        <v>0.5</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22">
+        <v>0.3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22">
+        <v>0.01</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0.05</v>
+      </c>
+      <c r="R22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="b">
+        <v>0</v>
+      </c>
+      <c r="U22" t="b">
+        <v>0</v>
+      </c>
+      <c r="V22" t="s">
+        <v>50</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+      <c r="X22" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>16</v>
+      </c>
+      <c r="AA22">
+        <v>1E-05</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>1E-08</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AE22">
+        <v>5</v>
+      </c>
+      <c r="AG22">
+        <v>0.4684228338486369</v>
+      </c>
+      <c r="AH22">
+        <v>0.4684228338486369</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23">
+        <v>128</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.105</v>
+      </c>
+      <c r="G23">
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23">
+        <v>0.3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>47</v>
+      </c>
+      <c r="L23">
+        <v>0.01</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0.05</v>
+      </c>
+      <c r="R23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="b">
+        <v>0</v>
+      </c>
+      <c r="U23" t="b">
+        <v>0</v>
+      </c>
+      <c r="V23" t="s">
+        <v>50</v>
+      </c>
+      <c r="W23" t="b">
+        <v>0</v>
+      </c>
+      <c r="X23" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>16</v>
+      </c>
+      <c r="AA23">
+        <v>1E-05</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>1E-08</v>
+      </c>
+      <c r="AD23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
+        <v>5</v>
+      </c>
+      <c r="AG23">
+        <v>0.4768825516422612</v>
+      </c>
+      <c r="AH23">
+        <v>0.4768825516422612</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK23">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>128</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.105</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24">
+        <v>0.3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L24">
+        <v>0.01</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0.05</v>
+      </c>
+      <c r="R24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" t="b">
+        <v>0</v>
+      </c>
+      <c r="U24" t="b">
+        <v>0</v>
+      </c>
+      <c r="V24" t="s">
+        <v>50</v>
+      </c>
+      <c r="W24" t="b">
+        <v>0</v>
+      </c>
+      <c r="X24" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>16</v>
+      </c>
+      <c r="AA24">
+        <v>1E-05</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>1E-08</v>
+      </c>
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AE24">
+        <v>5</v>
+      </c>
+      <c r="AG24">
+        <v>0.4707042761620226</v>
+      </c>
+      <c r="AH24">
+        <v>0.4707042761620226</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>128</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0.105</v>
+      </c>
+      <c r="G25">
+        <v>0.5</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25">
+        <v>0.3</v>
+      </c>
+      <c r="K25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L25">
+        <v>0.01</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0.05</v>
+      </c>
+      <c r="R25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25" t="b">
+        <v>0</v>
+      </c>
+      <c r="U25" t="b">
+        <v>0</v>
+      </c>
+      <c r="V25" t="s">
+        <v>50</v>
+      </c>
+      <c r="W25" t="b">
+        <v>0</v>
+      </c>
+      <c r="X25" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>16</v>
+      </c>
+      <c r="AA25">
+        <v>1E-05</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>1E-08</v>
+      </c>
+      <c r="AD25">
+        <v>1</v>
+      </c>
+      <c r="AE25">
+        <v>5</v>
+      </c>
+      <c r="AG25">
+        <v>0.4838860649382388</v>
+      </c>
+      <c r="AH25">
+        <v>0.4838860649382388</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>128</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0.105</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26">
+        <v>0.3</v>
+      </c>
+      <c r="K26" t="s">
+        <v>47</v>
+      </c>
+      <c r="L26">
+        <v>0.01</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0.05</v>
+      </c>
+      <c r="R26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" t="b">
+        <v>0</v>
+      </c>
+      <c r="U26" t="b">
+        <v>0</v>
+      </c>
+      <c r="V26" t="s">
+        <v>50</v>
+      </c>
+      <c r="W26" t="b">
+        <v>0</v>
+      </c>
+      <c r="X26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>16</v>
+      </c>
+      <c r="AA26">
+        <v>1E-05</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>1E-08</v>
+      </c>
+      <c r="AD26">
+        <v>1</v>
+      </c>
+      <c r="AE26">
+        <v>5</v>
+      </c>
+      <c r="AG26">
+        <v>0.4738659533516283</v>
+      </c>
+      <c r="AH26">
+        <v>0.4738659533516283</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>128</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.105</v>
+      </c>
+      <c r="G27">
+        <v>0.5</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27">
+        <v>0.3</v>
+      </c>
+      <c r="K27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L27">
+        <v>0.01</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0.05</v>
+      </c>
+      <c r="R27" t="b">
+        <v>0</v>
+      </c>
+      <c r="T27" t="b">
+        <v>0</v>
+      </c>
+      <c r="U27" t="b">
+        <v>0</v>
+      </c>
+      <c r="V27" t="s">
+        <v>50</v>
+      </c>
+      <c r="W27" t="b">
+        <v>0</v>
+      </c>
+      <c r="X27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>16</v>
+      </c>
+      <c r="AA27">
+        <v>1E-05</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>1E-08</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <v>5</v>
+      </c>
+      <c r="AG27">
+        <v>0.4806648190197469</v>
+      </c>
+      <c r="AH27">
+        <v>0.4806648190197469</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK27">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28">
+        <v>128</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0.105</v>
+      </c>
+      <c r="G28">
+        <v>0.5</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28">
+        <v>0.3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28">
+        <v>0.01</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0.05</v>
+      </c>
+      <c r="R28" t="b">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>49</v>
+      </c>
+      <c r="T28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U28" t="b">
+        <v>0</v>
+      </c>
+      <c r="V28" t="s">
+        <v>50</v>
+      </c>
+      <c r="W28" t="b">
+        <v>0</v>
+      </c>
+      <c r="X28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z28">
+        <v>16</v>
+      </c>
+      <c r="AA28">
+        <v>1E-05</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>1E-08</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <v>5</v>
+      </c>
+      <c r="AG28">
+        <v>0.4593320196055152</v>
+      </c>
+      <c r="AH28">
+        <v>0.5427824095978321</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29">
+        <v>128</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.105</v>
+      </c>
+      <c r="G29">
+        <v>0.5</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29">
+        <v>0.3</v>
+      </c>
+      <c r="K29" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29">
+        <v>0.01</v>
+      </c>
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0.05</v>
+      </c>
+      <c r="R29" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29" t="s">
+        <v>49</v>
+      </c>
+      <c r="T29" t="b">
+        <v>0</v>
+      </c>
+      <c r="U29" t="b">
+        <v>0</v>
+      </c>
+      <c r="V29" t="s">
+        <v>50</v>
+      </c>
+      <c r="W29" t="b">
+        <v>0</v>
+      </c>
+      <c r="X29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z29">
+        <v>16</v>
+      </c>
+      <c r="AA29">
+        <v>1E-05</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AC29">
+        <v>1E-08</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>5</v>
+      </c>
+      <c r="AG29">
+        <v>0.472590624022142</v>
+      </c>
+      <c r="AH29">
+        <v>0.5965473344148484</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK29">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>128</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0.105</v>
+      </c>
+      <c r="G30">
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30">
+        <v>0.3</v>
+      </c>
+      <c r="K30" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30">
+        <v>0.01</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0.05</v>
+      </c>
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" t="s">
+        <v>49</v>
+      </c>
+      <c r="T30" t="b">
+        <v>0</v>
+      </c>
+      <c r="U30" t="b">
+        <v>0</v>
+      </c>
+      <c r="V30" t="s">
+        <v>50</v>
+      </c>
+      <c r="W30" t="b">
+        <v>0</v>
+      </c>
+      <c r="X30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z30">
+        <v>16</v>
+      </c>
+      <c r="AA30">
+        <v>1E-05</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>1E-08</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AE30">
+        <v>5</v>
+      </c>
+      <c r="AG30">
+        <v>0.4857640834377365</v>
+      </c>
+      <c r="AH30">
+        <v>0.5744713747778639</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31">
+        <v>128</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0.105</v>
+      </c>
+      <c r="G31">
+        <v>0.5</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31">
+        <v>0.3</v>
+      </c>
+      <c r="K31" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31">
+        <v>0.01</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0.05</v>
+      </c>
+      <c r="R31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" t="s">
+        <v>49</v>
+      </c>
+      <c r="T31" t="b">
+        <v>0</v>
+      </c>
+      <c r="U31" t="b">
+        <v>0</v>
+      </c>
+      <c r="V31" t="s">
+        <v>50</v>
+      </c>
+      <c r="W31" t="b">
+        <v>0</v>
+      </c>
+      <c r="X31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z31">
+        <v>16</v>
+      </c>
+      <c r="AA31">
+        <v>1E-05</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <v>1E-08</v>
+      </c>
+      <c r="AD31">
+        <v>1</v>
+      </c>
+      <c r="AE31">
+        <v>5</v>
+      </c>
+      <c r="AG31">
+        <v>0.4682004331078098</v>
+      </c>
+      <c r="AH31">
+        <v>0.5514921355930711</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK31">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>128</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.105</v>
+      </c>
+      <c r="G32">
+        <v>0.5</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32">
+        <v>0.3</v>
+      </c>
+      <c r="K32" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32">
+        <v>0.01</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+      <c r="N32" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0.05</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" t="s">
+        <v>49</v>
+      </c>
+      <c r="T32" t="b">
+        <v>0</v>
+      </c>
+      <c r="U32" t="b">
+        <v>0</v>
+      </c>
+      <c r="V32" t="s">
+        <v>50</v>
+      </c>
+      <c r="W32" t="b">
+        <v>0</v>
+      </c>
+      <c r="X32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z32">
+        <v>16</v>
+      </c>
+      <c r="AA32">
+        <v>1E-05</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>1E-08</v>
+      </c>
+      <c r="AD32">
+        <v>1</v>
+      </c>
+      <c r="AE32">
+        <v>5</v>
+      </c>
+      <c r="AG32">
+        <v>0.4764352888223502</v>
+      </c>
+      <c r="AH32">
+        <v>0.5490202130648935</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33">
+        <v>128</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0.125</v>
+      </c>
+      <c r="G33">
+        <v>0.5</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="R33" t="b">
+        <v>0</v>
+      </c>
+      <c r="U33" t="b">
+        <v>0</v>
+      </c>
+      <c r="W33" t="b">
+        <v>0</v>
+      </c>
+      <c r="X33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>128</v>
+      </c>
+      <c r="AA33">
+        <v>1E-05</v>
+      </c>
+      <c r="AB33">
+        <v>0.01</v>
+      </c>
+      <c r="AC33">
+        <v>1E-08</v>
+      </c>
+      <c r="AD33">
+        <v>1</v>
+      </c>
+      <c r="AE33">
+        <v>5</v>
+      </c>
+      <c r="AF33">
+        <v>0.4058199569393488</v>
+      </c>
+      <c r="AH33">
+        <v>0.609046157025026</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>128</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0.125</v>
+      </c>
+      <c r="G34">
+        <v>0.5</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="R34" t="b">
+        <v>0</v>
+      </c>
+      <c r="U34" t="b">
+        <v>0</v>
+      </c>
+      <c r="W34" t="b">
+        <v>0</v>
+      </c>
+      <c r="X34" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>128</v>
+      </c>
+      <c r="AA34">
+        <v>1E-05</v>
+      </c>
+      <c r="AB34">
+        <v>0.01</v>
+      </c>
+      <c r="AC34">
+        <v>1E-08</v>
+      </c>
+      <c r="AD34">
+        <v>1</v>
+      </c>
+      <c r="AE34">
+        <v>5</v>
+      </c>
+      <c r="AF34">
+        <v>0.3954930782118511</v>
+      </c>
+      <c r="AH34">
+        <v>0.6074798951361772</v>
+      </c>
+      <c r="AI34" t="s">
         <v>84</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK34">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35">
+        <v>128</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.125</v>
+      </c>
+      <c r="G35">
+        <v>0.5</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>46</v>
+      </c>
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="R35" t="b">
+        <v>0</v>
+      </c>
+      <c r="U35" t="b">
+        <v>0</v>
+      </c>
+      <c r="W35" t="b">
+        <v>0</v>
+      </c>
+      <c r="X35" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>128</v>
+      </c>
+      <c r="AA35">
+        <v>1E-05</v>
+      </c>
+      <c r="AB35">
+        <v>0.01</v>
+      </c>
+      <c r="AC35">
+        <v>1E-08</v>
+      </c>
+      <c r="AD35">
+        <v>1</v>
+      </c>
+      <c r="AE35">
+        <v>5</v>
+      </c>
+      <c r="AF35">
+        <v>0.3860712387028176</v>
+      </c>
+      <c r="AH35">
+        <v>0.5910942650574863</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36">
+        <v>128</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.125</v>
+      </c>
+      <c r="G36">
+        <v>0.5</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36" t="s">
+        <v>46</v>
+      </c>
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36" t="b">
+        <v>0</v>
+      </c>
+      <c r="U36" t="b">
+        <v>0</v>
+      </c>
+      <c r="W36" t="b">
+        <v>0</v>
+      </c>
+      <c r="X36" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>128</v>
+      </c>
+      <c r="AA36">
+        <v>1E-05</v>
+      </c>
+      <c r="AB36">
+        <v>0.01</v>
+      </c>
+      <c r="AC36">
+        <v>1E-08</v>
+      </c>
+      <c r="AD36">
+        <v>1</v>
+      </c>
+      <c r="AE36">
+        <v>5</v>
+      </c>
+      <c r="AF36">
+        <v>0.3898129691058814</v>
+      </c>
+      <c r="AH36">
+        <v>0.6074982783720261</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK36">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37">
+        <v>128</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.125</v>
+      </c>
+      <c r="G37">
+        <v>0.5</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
+      <c r="U37" t="b">
+        <v>0</v>
+      </c>
+      <c r="W37" t="b">
+        <v>0</v>
+      </c>
+      <c r="X37" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>128</v>
+      </c>
+      <c r="AA37">
+        <v>1E-05</v>
+      </c>
+      <c r="AB37">
+        <v>0.01</v>
+      </c>
+      <c r="AC37">
+        <v>1E-08</v>
+      </c>
+      <c r="AD37">
+        <v>1</v>
+      </c>
+      <c r="AE37">
+        <v>5</v>
+      </c>
+      <c r="AF37">
+        <v>0.401672840367219</v>
+      </c>
+      <c r="AH37">
+        <v>0.6143510990665462</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK37">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38">
+        <v>128</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0.105</v>
+      </c>
+      <c r="G38">
+        <v>0.5</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38">
+        <v>0.3</v>
+      </c>
+      <c r="K38" t="s">
+        <v>47</v>
+      </c>
+      <c r="L38">
+        <v>0.01</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0.05</v>
+      </c>
+      <c r="R38" t="b">
+        <v>0</v>
+      </c>
+      <c r="T38" t="b">
+        <v>0</v>
+      </c>
+      <c r="U38" t="b">
+        <v>0</v>
+      </c>
+      <c r="V38" t="s">
+        <v>50</v>
+      </c>
+      <c r="W38" t="b">
+        <v>0</v>
+      </c>
+      <c r="X38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>16</v>
+      </c>
+      <c r="AA38">
+        <v>1E-05</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <v>1E-08</v>
+      </c>
+      <c r="AD38">
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <v>5</v>
+      </c>
+      <c r="AG38">
+        <v>0.4834330228414243</v>
+      </c>
+      <c r="AH38">
+        <v>0.5653439153439154</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK38">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39">
+        <v>128</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0.105</v>
+      </c>
+      <c r="G39">
+        <v>0.5</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39">
+        <v>0.3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39">
+        <v>0.01</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0.05</v>
+      </c>
+      <c r="R39" t="b">
+        <v>0</v>
+      </c>
+      <c r="T39" t="b">
+        <v>0</v>
+      </c>
+      <c r="U39" t="b">
+        <v>0</v>
+      </c>
+      <c r="V39" t="s">
+        <v>50</v>
+      </c>
+      <c r="W39" t="b">
+        <v>0</v>
+      </c>
+      <c r="X39" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <v>16</v>
+      </c>
+      <c r="AA39">
+        <v>1E-05</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39">
+        <v>1E-08</v>
+      </c>
+      <c r="AD39">
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <v>5</v>
+      </c>
+      <c r="AG39">
+        <v>0.4714363399136356</v>
+      </c>
+      <c r="AH39">
+        <v>0.5644254065099296</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40">
+        <v>128</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.105</v>
+      </c>
+      <c r="G40">
+        <v>0.5</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40">
+        <v>0.3</v>
+      </c>
+      <c r="K40" t="s">
+        <v>47</v>
+      </c>
+      <c r="L40">
+        <v>0.01</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0.05</v>
+      </c>
+      <c r="R40" t="b">
+        <v>0</v>
+      </c>
+      <c r="T40" t="b">
+        <v>0</v>
+      </c>
+      <c r="U40" t="b">
+        <v>0</v>
+      </c>
+      <c r="V40" t="s">
+        <v>50</v>
+      </c>
+      <c r="W40" t="b">
+        <v>0</v>
+      </c>
+      <c r="X40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z40">
+        <v>16</v>
+      </c>
+      <c r="AA40">
+        <v>1E-05</v>
+      </c>
+      <c r="AB40">
+        <v>0</v>
+      </c>
+      <c r="AC40">
+        <v>1E-08</v>
+      </c>
+      <c r="AD40">
+        <v>1</v>
+      </c>
+      <c r="AE40">
+        <v>5</v>
+      </c>
+      <c r="AG40">
+        <v>0.5070068072489867</v>
+      </c>
+      <c r="AH40">
+        <v>0.5727848700085458</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK40">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41">
+        <v>128</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0.105</v>
+      </c>
+      <c r="G41">
+        <v>0.5</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41">
+        <v>0.3</v>
+      </c>
+      <c r="K41" t="s">
+        <v>47</v>
+      </c>
+      <c r="L41">
+        <v>0.01</v>
+      </c>
+      <c r="M41">
+        <v>3</v>
+      </c>
+      <c r="N41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" t="b">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0.05</v>
+      </c>
+      <c r="R41" t="b">
+        <v>0</v>
+      </c>
+      <c r="T41" t="b">
+        <v>0</v>
+      </c>
+      <c r="U41" t="b">
+        <v>0</v>
+      </c>
+      <c r="V41" t="s">
+        <v>50</v>
+      </c>
+      <c r="W41" t="b">
+        <v>0</v>
+      </c>
+      <c r="X41" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>16</v>
+      </c>
+      <c r="AA41">
+        <v>1E-05</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
+      <c r="AC41">
+        <v>1E-08</v>
+      </c>
+      <c r="AD41">
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <v>5</v>
+      </c>
+      <c r="AG41">
+        <v>0.5695639875996646</v>
+      </c>
+      <c r="AH41">
+        <v>0.5986787818849619</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK41">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42">
+        <v>128</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0.105</v>
+      </c>
+      <c r="G42">
+        <v>0.5</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42">
+        <v>0.3</v>
+      </c>
+      <c r="K42" t="s">
+        <v>47</v>
+      </c>
+      <c r="L42">
+        <v>0.01</v>
+      </c>
+      <c r="M42">
+        <v>3</v>
+      </c>
+      <c r="N42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" t="b">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0.05</v>
+      </c>
+      <c r="R42" t="b">
+        <v>0</v>
+      </c>
+      <c r="T42" t="b">
+        <v>0</v>
+      </c>
+      <c r="U42" t="b">
+        <v>0</v>
+      </c>
+      <c r="V42" t="s">
+        <v>50</v>
+      </c>
+      <c r="W42" t="b">
+        <v>0</v>
+      </c>
+      <c r="X42" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>16</v>
+      </c>
+      <c r="AA42">
+        <v>1E-05</v>
+      </c>
+      <c r="AB42">
+        <v>0</v>
+      </c>
+      <c r="AC42">
+        <v>1E-08</v>
+      </c>
+      <c r="AD42">
+        <v>1</v>
+      </c>
+      <c r="AE42">
+        <v>5</v>
+      </c>
+      <c r="AG42">
+        <v>0.468034707105281</v>
+      </c>
+      <c r="AH42">
+        <v>0.5465946161700393</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43">
+        <v>128</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0.105</v>
+      </c>
+      <c r="G43">
+        <v>0.5</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43">
+        <v>0.3</v>
+      </c>
+      <c r="K43" t="s">
+        <v>47</v>
+      </c>
+      <c r="L43">
+        <v>0.01</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43" t="b">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0.05</v>
+      </c>
+      <c r="R43" t="b">
+        <v>0</v>
+      </c>
+      <c r="T43" t="b">
+        <v>0</v>
+      </c>
+      <c r="U43" t="b">
+        <v>0</v>
+      </c>
+      <c r="V43" t="s">
+        <v>50</v>
+      </c>
+      <c r="W43" t="b">
+        <v>0</v>
+      </c>
+      <c r="X43" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>16</v>
+      </c>
+      <c r="AA43">
+        <v>1E-05</v>
+      </c>
+      <c r="AB43">
+        <v>0</v>
+      </c>
+      <c r="AC43">
+        <v>1E-08</v>
+      </c>
+      <c r="AD43">
+        <v>1</v>
+      </c>
+      <c r="AE43">
+        <v>5</v>
+      </c>
+      <c r="AG43">
+        <v>0.4986878536557414</v>
+      </c>
+      <c r="AH43">
+        <v>0.5868311116139943</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>128</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0.105</v>
+      </c>
+      <c r="G44">
+        <v>0.5</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44">
+        <v>0.3</v>
+      </c>
+      <c r="K44" t="s">
+        <v>47</v>
+      </c>
+      <c r="L44">
+        <v>0.01</v>
+      </c>
+      <c r="M44">
+        <v>3</v>
+      </c>
+      <c r="N44" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44" t="b">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0.05</v>
+      </c>
+      <c r="R44" t="b">
+        <v>0</v>
+      </c>
+      <c r="T44" t="b">
+        <v>0</v>
+      </c>
+      <c r="U44" t="b">
+        <v>0</v>
+      </c>
+      <c r="V44" t="s">
+        <v>50</v>
+      </c>
+      <c r="W44" t="b">
+        <v>0</v>
+      </c>
+      <c r="X44" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <v>16</v>
+      </c>
+      <c r="AA44">
+        <v>1E-05</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
+      </c>
+      <c r="AC44">
+        <v>1E-08</v>
+      </c>
+      <c r="AD44">
+        <v>1</v>
+      </c>
+      <c r="AE44">
+        <v>5</v>
+      </c>
+      <c r="AG44">
+        <v>0.4773349776838149</v>
+      </c>
+      <c r="AH44">
+        <v>0.571145443984855</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK44">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <v>128</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0.105</v>
+      </c>
+      <c r="G45">
+        <v>0.5</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45">
+        <v>0.3</v>
+      </c>
+      <c r="K45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L45">
+        <v>0.01</v>
+      </c>
+      <c r="M45">
+        <v>3</v>
+      </c>
+      <c r="N45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45" t="b">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0.05</v>
+      </c>
+      <c r="R45" t="b">
+        <v>0</v>
+      </c>
+      <c r="T45" t="b">
+        <v>0</v>
+      </c>
+      <c r="U45" t="b">
+        <v>0</v>
+      </c>
+      <c r="V45" t="s">
+        <v>50</v>
+      </c>
+      <c r="W45" t="b">
+        <v>0</v>
+      </c>
+      <c r="X45" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>16</v>
+      </c>
+      <c r="AA45">
+        <v>1E-05</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
+      </c>
+      <c r="AC45">
+        <v>1E-08</v>
+      </c>
+      <c r="AD45">
+        <v>1</v>
+      </c>
+      <c r="AE45">
+        <v>5</v>
+      </c>
+      <c r="AG45">
+        <v>0.4821491251812839</v>
+      </c>
+      <c r="AH45">
+        <v>0.5657308488509448</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK45">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>